<commit_message>
added new WIP walk cycle, currently not used tho
</commit_message>
<xml_diff>
--- a/documentation/animations.xlsx
+++ b/documentation/animations.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="81">
   <si>
     <t>good motion needs: on-the-ground pushing motion, weight handoff, and midair reposition</t>
   </si>
@@ -182,6 +182,81 @@
   </si>
   <si>
     <t>TODO: side-walk sequence, maybe</t>
+  </si>
+  <si>
+    <t>side: 6 positions</t>
+  </si>
+  <si>
+    <t>side_neutral</t>
+  </si>
+  <si>
+    <t>side_neutral_up</t>
+  </si>
+  <si>
+    <t>side_left_up</t>
+  </si>
+  <si>
+    <t>side_right_up</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>corner: 10 positions</t>
+  </si>
+  <si>
+    <t>corn_neutral</t>
+  </si>
+  <si>
+    <t>corn_neutral_up</t>
+  </si>
+  <si>
+    <t>corn_leftin</t>
+  </si>
+  <si>
+    <t>corn_leftout</t>
+  </si>
+  <si>
+    <t>corn_leftin_up</t>
+  </si>
+  <si>
+    <t>corn_leftout_up</t>
+  </si>
+  <si>
+    <t>corn_rightin</t>
+  </si>
+  <si>
+    <t>corn_rightout</t>
+  </si>
+  <si>
+    <t>corn_rightin_up</t>
+  </si>
+  <si>
+    <t>corn_rightout_up</t>
+  </si>
+  <si>
+    <t>*NEW_RIGHT_NEUTRAL_LEFT_UP_NEUTRAL</t>
+  </si>
+  <si>
+    <t>NEW_RIGHT_BACK_LEFT_UP_FORWARD</t>
+  </si>
+  <si>
+    <t>NEW_RIGHT_BACK_LEFT_FORWARD</t>
+  </si>
+  <si>
+    <t>NEW_RIGHT_UP_BACK_LEFT_FORWARD</t>
+  </si>
+  <si>
+    <t>*NEW_RIGHT_UP_NEUTRAL_LEFT_NEUTRAL</t>
+  </si>
+  <si>
+    <t>NEW_RIGHT_UP_FORWARD_LEFT_BACK</t>
+  </si>
+  <si>
+    <t>NEW_RIGHT_FORWARD_LEFT_BACK</t>
+  </si>
+  <si>
+    <t>NEW_RIGHT_FORWARD_LEFT_UP_BACK</t>
   </si>
 </sst>
 </file>
@@ -211,13 +286,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -241,34 +310,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -281,6 +334,22 @@
     <font>
       <b/>
       <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -309,9 +378,45 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -324,38 +429,8 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="36">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -382,37 +457,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -430,7 +583,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -442,12 +595,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -460,7 +607,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -472,6 +619,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -479,90 +632,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -576,11 +645,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -618,28 +693,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -659,17 +723,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -678,152 +747,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -840,6 +909,21 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1161,10 +1245,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I84"/>
+  <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -1478,9 +1562,7 @@
     </row>
     <row r="31" customFormat="1" spans="3:7">
       <c r="C31" s="3"/>
-      <c r="D31"/>
       <c r="E31" s="3"/>
-      <c r="F31"/>
       <c r="G31" s="3"/>
     </row>
     <row r="32" spans="1:9">
@@ -1930,7 +2012,6 @@
     </row>
     <row r="73" spans="3:7">
       <c r="C73" s="1"/>
-      <c r="D73"/>
       <c r="F73" s="2"/>
       <c r="G73" s="1"/>
     </row>
@@ -1989,6 +2070,466 @@
     <row r="84" spans="2:2">
       <c r="B84" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="86" spans="2:8">
+      <c r="B86" t="s">
+        <v>56</v>
+      </c>
+      <c r="C86" t="s">
+        <v>57</v>
+      </c>
+      <c r="D86" t="s">
+        <v>58</v>
+      </c>
+      <c r="E86" t="s">
+        <v>46</v>
+      </c>
+      <c r="F86" t="s">
+        <v>59</v>
+      </c>
+      <c r="G86" t="s">
+        <v>53</v>
+      </c>
+      <c r="H86" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="87" spans="3:4">
+      <c r="C87" t="s">
+        <v>61</v>
+      </c>
+      <c r="D87" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="88" spans="2:12">
+      <c r="B88" t="s">
+        <v>62</v>
+      </c>
+      <c r="C88" t="s">
+        <v>63</v>
+      </c>
+      <c r="D88" t="s">
+        <v>64</v>
+      </c>
+      <c r="E88" t="s">
+        <v>65</v>
+      </c>
+      <c r="F88" t="s">
+        <v>66</v>
+      </c>
+      <c r="G88" t="s">
+        <v>67</v>
+      </c>
+      <c r="H88" t="s">
+        <v>68</v>
+      </c>
+      <c r="I88" t="s">
+        <v>69</v>
+      </c>
+      <c r="J88" t="s">
+        <v>70</v>
+      </c>
+      <c r="K88" t="s">
+        <v>71</v>
+      </c>
+      <c r="L88" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3">
+      <c r="B93" t="s">
+        <v>10</v>
+      </c>
+      <c r="C93" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="94" spans="3:8">
+      <c r="C94" t="s">
+        <v>12</v>
+      </c>
+      <c r="D94" t="s">
+        <v>13</v>
+      </c>
+      <c r="E94" t="s">
+        <v>14</v>
+      </c>
+      <c r="F94" t="s">
+        <v>15</v>
+      </c>
+      <c r="G94" t="s">
+        <v>16</v>
+      </c>
+      <c r="H94" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8">
+      <c r="A96">
+        <v>31</v>
+      </c>
+      <c r="B96" t="s">
+        <v>18</v>
+      </c>
+      <c r="C96" t="s">
+        <v>19</v>
+      </c>
+      <c r="D96" t="s">
+        <v>19</v>
+      </c>
+      <c r="E96" t="s">
+        <v>19</v>
+      </c>
+      <c r="F96" t="s">
+        <v>19</v>
+      </c>
+      <c r="G96" t="s">
+        <v>19</v>
+      </c>
+      <c r="H96" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8">
+      <c r="A99">
+        <v>132</v>
+      </c>
+      <c r="B99" t="s">
+        <v>73</v>
+      </c>
+      <c r="C99" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D99" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E99" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F99" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G99" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H99" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="100" spans="3:8">
+      <c r="C100" s="7"/>
+      <c r="D100" s="8"/>
+      <c r="E100" s="7"/>
+      <c r="F100" s="8"/>
+      <c r="G100" s="7"/>
+      <c r="H100" s="8"/>
+    </row>
+    <row r="101" spans="1:8">
+      <c r="A101">
+        <v>133</v>
+      </c>
+      <c r="B101" t="s">
+        <v>74</v>
+      </c>
+      <c r="C101" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D101" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E101" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F101" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G101" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H101" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="102" spans="3:8">
+      <c r="C102" s="9"/>
+      <c r="D102" s="10"/>
+      <c r="E102" s="9"/>
+      <c r="F102" s="10"/>
+      <c r="G102" s="9"/>
+      <c r="H102" s="10"/>
+    </row>
+    <row r="103" spans="1:8">
+      <c r="A103">
+        <v>134</v>
+      </c>
+      <c r="B103" t="s">
+        <v>75</v>
+      </c>
+      <c r="C103" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D103" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E103" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F103" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G103" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H103" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="104" spans="3:8">
+      <c r="C104" s="10"/>
+      <c r="D104" s="9"/>
+      <c r="E104" s="10"/>
+      <c r="F104" s="9"/>
+      <c r="G104" s="10"/>
+      <c r="H104" s="9"/>
+    </row>
+    <row r="105" spans="1:8">
+      <c r="A105">
+        <v>135</v>
+      </c>
+      <c r="B105" t="s">
+        <v>76</v>
+      </c>
+      <c r="C105" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D105" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E105" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F105" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G105" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H105" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="106" spans="3:8">
+      <c r="C106" s="8"/>
+      <c r="D106" s="7"/>
+      <c r="E106" s="8"/>
+      <c r="F106" s="7"/>
+      <c r="G106" s="8"/>
+      <c r="H106" s="7"/>
+    </row>
+    <row r="107" spans="1:8">
+      <c r="A107">
+        <v>136</v>
+      </c>
+      <c r="B107" t="s">
+        <v>77</v>
+      </c>
+      <c r="C107" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D107" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E107" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F107" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G107" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H107" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="108" spans="3:8">
+      <c r="C108" s="8"/>
+      <c r="D108" s="7"/>
+      <c r="E108" s="8"/>
+      <c r="F108" s="7"/>
+      <c r="G108" s="8"/>
+      <c r="H108" s="7"/>
+    </row>
+    <row r="109" spans="1:8">
+      <c r="A109">
+        <v>137</v>
+      </c>
+      <c r="B109" t="s">
+        <v>78</v>
+      </c>
+      <c r="C109" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D109" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E109" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F109" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G109" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H109" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="110" spans="3:8">
+      <c r="C110" s="10"/>
+      <c r="D110" s="9"/>
+      <c r="E110" s="10"/>
+      <c r="F110" s="9"/>
+      <c r="G110" s="10"/>
+      <c r="H110" s="9"/>
+    </row>
+    <row r="111" spans="1:8">
+      <c r="A111">
+        <v>138</v>
+      </c>
+      <c r="B111" t="s">
+        <v>79</v>
+      </c>
+      <c r="C111" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D111" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E111" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F111" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G111" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H111" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="112" spans="3:8">
+      <c r="C112" s="9"/>
+      <c r="D112" s="10"/>
+      <c r="E112" s="9"/>
+      <c r="F112" s="10"/>
+      <c r="G112" s="9"/>
+      <c r="H112" s="10"/>
+    </row>
+    <row r="113" spans="1:8">
+      <c r="A113">
+        <v>139</v>
+      </c>
+      <c r="B113" t="s">
+        <v>80</v>
+      </c>
+      <c r="C113" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D113" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E113" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F113" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G113" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H113" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="114" spans="3:8">
+      <c r="C114" s="7"/>
+      <c r="D114" s="8"/>
+      <c r="E114" s="7"/>
+      <c r="F114" s="8"/>
+      <c r="G114" s="7"/>
+      <c r="H114" s="8"/>
+    </row>
+    <row r="115" spans="1:8">
+      <c r="A115">
+        <v>132</v>
+      </c>
+      <c r="B115" t="s">
+        <v>73</v>
+      </c>
+      <c r="C115" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D115" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E115" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F115" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G115" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H115" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="116" spans="3:8">
+      <c r="C116" s="9"/>
+      <c r="D116" s="9"/>
+      <c r="E116" s="9"/>
+      <c r="F116" s="9"/>
+      <c r="G116" s="9"/>
+      <c r="H116" s="9"/>
+    </row>
+    <row r="117" spans="3:8">
+      <c r="C117" s="9"/>
+      <c r="D117" s="9"/>
+      <c r="E117" s="9"/>
+      <c r="F117" s="9"/>
+      <c r="G117" s="9"/>
+      <c r="H117" s="9"/>
+    </row>
+    <row r="118" spans="1:8">
+      <c r="A118">
+        <v>31</v>
+      </c>
+      <c r="B118" t="s">
+        <v>18</v>
+      </c>
+      <c r="C118" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D118" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E118" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F118" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G118" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H118" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added current crab-walk and ideal crab-walk
</commit_message>
<xml_diff>
--- a/documentation/animations.xlsx
+++ b/documentation/animations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22488" windowHeight="9204"/>
+    <workbookView windowWidth="10968" windowHeight="8940" tabRatio="358"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="123">
   <si>
     <t>good motion needs: on-the-ground pushing motion, weight handoff, and midair reposition</t>
   </si>
@@ -124,21 +124,21 @@
     <t>TALL_TRI_RIGHT_LEFT_LEFT_UP_RIGHT</t>
   </si>
   <si>
+    <t>THIS IS THE ORIGINAL WALK-CYCLE TABLE BEFORE BRIAN BEGAN WORKING</t>
+  </si>
+  <si>
+    <t>seems nonsensical like it shouldn't work at all... using only half-motion and out of sync</t>
+  </si>
+  <si>
+    <t>theory: maybe with original drivers the full-range pushing was too jerky so they switched to this method? that cant be right....</t>
+  </si>
+  <si>
+    <t>why would they design it like this?</t>
+  </si>
+  <si>
     <t>walk cycle: LEG_TALL_MOVEMENT_TABLE, sides need different poses than the other "corner" legs but its all in the same table</t>
   </si>
   <si>
-    <t>THIS IS THE ORIGINAL WALK-CYCLE TABLE BEFORE BRIAN BEGAN WORKING</t>
-  </si>
-  <si>
-    <t>seems nonsensical like it shouldn't work at all... using only half-motion and out of sync</t>
-  </si>
-  <si>
-    <t>theory: maybe with original drivers the full-range pushing was too jerky so they switched to this method? that cant be right....</t>
-  </si>
-  <si>
-    <t>why would they design it like this?</t>
-  </si>
-  <si>
     <t>TALL_TRI_RIGHT_BACK_LEFT_UP_FORWARD</t>
   </si>
   <si>
@@ -181,82 +181,208 @@
     <t>TALL_TRI_RIGHT_FORWARD_LEFT_UP_BACK</t>
   </si>
   <si>
-    <t>TODO: side-walk sequence, maybe</t>
-  </si>
-  <si>
-    <t>side: 6 positions</t>
+    <t>NEW* WALK-CYCLE</t>
+  </si>
+  <si>
+    <t>this is the table for brian's new forward-walk cycle. currently doesn't work, needs much more tuning and adjusting, but is theoretically superior to the above</t>
+  </si>
+  <si>
+    <t>this uses full-range motion on all legs, and many of the poses can be re-used in the crab-walk below</t>
+  </si>
+  <si>
+    <t>walk cycle: LEG_NEW_MOVEMENT_TABLE</t>
+  </si>
+  <si>
+    <t>*NEW_RIGHT_NEUTRAL_LEFT_UP_NEUTRAL</t>
+  </si>
+  <si>
+    <t>corn_neutral</t>
+  </si>
+  <si>
+    <t>side_neutral_up</t>
+  </si>
+  <si>
+    <t>corn_neutral_up</t>
   </si>
   <si>
     <t>side_neutral</t>
   </si>
   <si>
-    <t>side_neutral_up</t>
+    <t>NEW_RIGHT_BACK_LEFT_UP_FORWARD</t>
+  </si>
+  <si>
+    <t>corn_rightin</t>
   </si>
   <si>
     <t>side_left_up</t>
   </si>
   <si>
+    <t>corn_rightout</t>
+  </si>
+  <si>
+    <t>corn_rightin_up</t>
+  </si>
+  <si>
+    <t>corn_rightout_up</t>
+  </si>
+  <si>
+    <t>NEW_RIGHT_BACK_LEFT_FORWARD</t>
+  </si>
+  <si>
+    <t>NEW_RIGHT_UP_BACK_LEFT_FORWARD</t>
+  </si>
+  <si>
+    <t>*NEW_RIGHT_UP_NEUTRAL_LEFT_NEUTRAL</t>
+  </si>
+  <si>
+    <t>NEW_RIGHT_UP_FORWARD_LEFT_BACK</t>
+  </si>
+  <si>
+    <t>corn_leftout_up</t>
+  </si>
+  <si>
+    <t>corn_leftin_up</t>
+  </si>
+  <si>
+    <t>corn_leftout</t>
+  </si>
+  <si>
     <t>side_right_up</t>
   </si>
   <si>
-    <t>*</t>
-  </si>
-  <si>
-    <t>corner: 10 positions</t>
-  </si>
-  <si>
-    <t>corn_neutral</t>
-  </si>
-  <si>
-    <t>corn_neutral_up</t>
-  </si>
-  <si>
     <t>corn_leftin</t>
   </si>
   <si>
-    <t>corn_leftout</t>
-  </si>
-  <si>
-    <t>corn_leftin_up</t>
-  </si>
-  <si>
-    <t>corn_leftout_up</t>
-  </si>
-  <si>
-    <t>corn_rightin</t>
-  </si>
-  <si>
-    <t>corn_rightout</t>
-  </si>
-  <si>
-    <t>corn_rightin_up</t>
-  </si>
-  <si>
-    <t>corn_rightout_up</t>
-  </si>
-  <si>
-    <t>*NEW_RIGHT_NEUTRAL_LEFT_UP_NEUTRAL</t>
-  </si>
-  <si>
-    <t>NEW_RIGHT_BACK_LEFT_UP_FORWARD</t>
-  </si>
-  <si>
-    <t>NEW_RIGHT_BACK_LEFT_FORWARD</t>
-  </si>
-  <si>
-    <t>NEW_RIGHT_UP_BACK_LEFT_FORWARD</t>
-  </si>
-  <si>
-    <t>*NEW_RIGHT_UP_NEUTRAL_LEFT_NEUTRAL</t>
-  </si>
-  <si>
-    <t>NEW_RIGHT_UP_FORWARD_LEFT_BACK</t>
-  </si>
-  <si>
     <t>NEW_RIGHT_FORWARD_LEFT_BACK</t>
   </si>
   <si>
     <t>NEW_RIGHT_FORWARD_LEFT_UP_BACK</t>
+  </si>
+  <si>
+    <t>CRAB-WALK CYCLE</t>
+  </si>
+  <si>
+    <t>this is the original crab-walk cycle from before Brian started making changes</t>
+  </si>
+  <si>
+    <t>crab-cycle: LEG_TALL_SIDE_MOVEMENT_TABLE</t>
+  </si>
+  <si>
+    <t>walking in the FR direction</t>
+  </si>
+  <si>
+    <t>TALL_TRI_FRONT_CENTER_UP_OUT_BACK_NEUTRAL</t>
+  </si>
+  <si>
+    <t>center_out_up</t>
+  </si>
+  <si>
+    <t>center_neutral</t>
+  </si>
+  <si>
+    <t>TALL_TRI_FRONT_CENTER_OUT_BACK_UP_NEUTRAL</t>
+  </si>
+  <si>
+    <t>center_out</t>
+  </si>
+  <si>
+    <t>center_neutral_up</t>
+  </si>
+  <si>
+    <t>TALL_TRI_FRONT_BACKWARDS_BACK_UP_NEUTRAL</t>
+  </si>
+  <si>
+    <t>side_out_right</t>
+  </si>
+  <si>
+    <t>side_out_left</t>
+  </si>
+  <si>
+    <t>TALL_TRI_FRONT_BACKWARDS_BACK_NEUTRAL</t>
+  </si>
+  <si>
+    <t>*TALL_TRI_FRONT_UP_NEUTRAL_BACK_NEUTRAL</t>
+  </si>
+  <si>
+    <t>TALL_TRI_FRONT_UP_NEUTRAL_BACK_BACKWARDS</t>
+  </si>
+  <si>
+    <t>TALL_TRI_FRONT_NEUTRAL_BACK_BACKWARDS</t>
+  </si>
+  <si>
+    <t>*TALL_TRI_FRONT_NEUTRAL_BACK_UP_NEUTRAL</t>
+  </si>
+  <si>
+    <t>CRAB-WALK CYCLE 2</t>
+  </si>
+  <si>
+    <t>this is the improved crab-walk cycle from Brian</t>
+  </si>
+  <si>
+    <t>theoretically superior due to using full-range motion, but we'll see</t>
+  </si>
+  <si>
+    <t>walking in the R direction</t>
+  </si>
+  <si>
+    <t>"side_" poses correspond to "corn_" poses from new walk-cycle</t>
+  </si>
+  <si>
+    <t>*a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>side_rightout_up</t>
+  </si>
+  <si>
+    <t>center_in</t>
+  </si>
+  <si>
+    <t>side_leftout_up</t>
+  </si>
+  <si>
+    <t>side_rightout</t>
+  </si>
+  <si>
+    <t>side_leftout</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>center_in_up</t>
+  </si>
+  <si>
+    <t>*e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>side_leftin</t>
+  </si>
+  <si>
+    <t>side_rightin</t>
+  </si>
+  <si>
+    <t>side_leftin_up</t>
+  </si>
+  <si>
+    <t>side_rightin_up</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>center_out_down</t>
+  </si>
+  <si>
+    <t>h</t>
   </si>
 </sst>
 </file>
@@ -264,10 +390,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -288,15 +414,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -310,8 +435,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -326,7 +460,58 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -348,67 +533,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -469,13 +595,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -487,7 +613,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -499,7 +697,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -523,13 +733,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -541,97 +751,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -642,21 +768,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -675,35 +786,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -726,8 +819,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -742,12 +835,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -765,134 +891,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -918,9 +1044,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
@@ -1245,10 +1368,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L118"/>
+  <dimension ref="A1:I211"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A179" workbookViewId="0">
+      <selection activeCell="B174" sqref="B174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -1688,28 +1811,28 @@
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="2:2">
-      <c r="B44" t="s">
-        <v>36</v>
-      </c>
-    </row>
     <row r="45" spans="2:2">
       <c r="B45" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="2:2">
       <c r="B46" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="2:2">
       <c r="B47" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="2:2">
       <c r="B48" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2067,75 +2190,24 @@
         <v>19</v>
       </c>
     </row>
-    <row r="84" spans="2:2">
-      <c r="B84" t="s">
+    <row r="85" spans="2:2">
+      <c r="B85" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="86" spans="2:8">
+    <row r="86" spans="2:2">
       <c r="B86" t="s">
         <v>56</v>
       </c>
-      <c r="C86" t="s">
+    </row>
+    <row r="87" spans="2:2">
+      <c r="B87" t="s">
         <v>57</v>
       </c>
-      <c r="D86" t="s">
+    </row>
+    <row r="88" spans="2:2">
+      <c r="B88" t="s">
         <v>58</v>
-      </c>
-      <c r="E86" t="s">
-        <v>46</v>
-      </c>
-      <c r="F86" t="s">
-        <v>59</v>
-      </c>
-      <c r="G86" t="s">
-        <v>53</v>
-      </c>
-      <c r="H86" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="87" spans="3:4">
-      <c r="C87" t="s">
-        <v>61</v>
-      </c>
-      <c r="D87" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="88" spans="2:12">
-      <c r="B88" t="s">
-        <v>62</v>
-      </c>
-      <c r="C88" t="s">
-        <v>63</v>
-      </c>
-      <c r="D88" t="s">
-        <v>64</v>
-      </c>
-      <c r="E88" t="s">
-        <v>65</v>
-      </c>
-      <c r="F88" t="s">
-        <v>66</v>
-      </c>
-      <c r="G88" t="s">
-        <v>67</v>
-      </c>
-      <c r="H88" t="s">
-        <v>68</v>
-      </c>
-      <c r="I88" t="s">
-        <v>69</v>
-      </c>
-      <c r="J88" t="s">
-        <v>70</v>
-      </c>
-      <c r="K88" t="s">
-        <v>71</v>
-      </c>
-      <c r="L88" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="93" spans="2:3">
@@ -2197,25 +2269,25 @@
         <v>132</v>
       </c>
       <c r="B99" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="C99" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D99" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E99" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F99" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G99" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D99" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E99" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="F99" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="G99" s="6" t="s">
-        <v>57</v>
-      </c>
       <c r="H99" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="100" spans="3:8">
@@ -2231,93 +2303,93 @@
         <v>133</v>
       </c>
       <c r="B101" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F101" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G101" s="6" t="s">
         <v>46</v>
       </c>
       <c r="H101" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="102" spans="3:8">
-      <c r="C102" s="9"/>
-      <c r="D102" s="10"/>
-      <c r="E102" s="9"/>
-      <c r="F102" s="10"/>
-      <c r="G102" s="9"/>
-      <c r="H102" s="10"/>
+      <c r="C102" s="6"/>
+      <c r="D102" s="9"/>
+      <c r="E102" s="6"/>
+      <c r="F102" s="9"/>
+      <c r="G102" s="6"/>
+      <c r="H102" s="9"/>
     </row>
     <row r="103" spans="1:8">
       <c r="A103">
         <v>134</v>
       </c>
       <c r="B103" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D103" s="6" t="s">
         <v>46</v>
       </c>
       <c r="E103" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F103" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G103" s="6" t="s">
         <v>46</v>
       </c>
       <c r="H103" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="104" spans="3:8">
-      <c r="C104" s="10"/>
-      <c r="D104" s="9"/>
-      <c r="E104" s="10"/>
-      <c r="F104" s="9"/>
-      <c r="G104" s="10"/>
-      <c r="H104" s="9"/>
+      <c r="C104" s="9"/>
+      <c r="D104" s="6"/>
+      <c r="E104" s="9"/>
+      <c r="F104" s="6"/>
+      <c r="G104" s="9"/>
+      <c r="H104" s="6"/>
     </row>
     <row r="105" spans="1:8">
       <c r="A105">
         <v>135</v>
       </c>
       <c r="B105" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D105" s="6" t="s">
         <v>46</v>
       </c>
       <c r="E105" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F105" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G105" s="6" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="H105" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="106" spans="3:8">
@@ -2333,25 +2405,25 @@
         <v>136</v>
       </c>
       <c r="B107" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E107" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F107" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G107" s="6" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="H107" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="108" spans="3:8">
@@ -2367,34 +2439,34 @@
         <v>137</v>
       </c>
       <c r="B109" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D109" s="6" t="s">
         <v>53</v>
       </c>
       <c r="E109" s="6" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="F109" s="6" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="G109" s="6" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="H109" s="6" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
     </row>
     <row r="110" spans="3:8">
-      <c r="C110" s="10"/>
-      <c r="D110" s="9"/>
-      <c r="E110" s="10"/>
-      <c r="F110" s="9"/>
-      <c r="G110" s="10"/>
-      <c r="H110" s="9"/>
+      <c r="C110" s="9"/>
+      <c r="D110" s="6"/>
+      <c r="E110" s="9"/>
+      <c r="F110" s="6"/>
+      <c r="G110" s="9"/>
+      <c r="H110" s="6"/>
     </row>
     <row r="111" spans="1:8">
       <c r="A111">
@@ -2404,31 +2476,31 @@
         <v>79</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="D111" s="6" t="s">
         <v>53</v>
       </c>
       <c r="E111" s="6" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="F111" s="6" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="G111" s="6" t="s">
         <v>53</v>
       </c>
       <c r="H111" s="6" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
     </row>
     <row r="112" spans="3:8">
-      <c r="C112" s="9"/>
-      <c r="D112" s="10"/>
-      <c r="E112" s="9"/>
-      <c r="F112" s="10"/>
-      <c r="G112" s="9"/>
-      <c r="H112" s="10"/>
+      <c r="C112" s="6"/>
+      <c r="D112" s="9"/>
+      <c r="E112" s="6"/>
+      <c r="F112" s="9"/>
+      <c r="G112" s="6"/>
+      <c r="H112" s="9"/>
     </row>
     <row r="113" spans="1:8">
       <c r="A113">
@@ -2438,22 +2510,22 @@
         <v>80</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="D113" s="6" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="E113" s="6" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="F113" s="6" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="G113" s="6" t="s">
         <v>53</v>
       </c>
       <c r="H113" s="6" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
     </row>
     <row r="114" spans="3:8">
@@ -2469,42 +2541,42 @@
         <v>132</v>
       </c>
       <c r="B115" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="C115" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D115" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E115" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F115" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G115" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D115" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E115" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="F115" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="G115" s="6" t="s">
-        <v>57</v>
-      </c>
       <c r="H115" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="116" spans="3:8">
-      <c r="C116" s="9"/>
-      <c r="D116" s="9"/>
-      <c r="E116" s="9"/>
-      <c r="F116" s="9"/>
-      <c r="G116" s="9"/>
-      <c r="H116" s="9"/>
+      <c r="C116" s="6"/>
+      <c r="D116" s="6"/>
+      <c r="E116" s="6"/>
+      <c r="F116" s="6"/>
+      <c r="G116" s="6"/>
+      <c r="H116" s="6"/>
     </row>
     <row r="117" spans="3:8">
-      <c r="C117" s="9"/>
-      <c r="D117" s="9"/>
-      <c r="E117" s="9"/>
-      <c r="F117" s="9"/>
-      <c r="G117" s="9"/>
-      <c r="H117" s="9"/>
+      <c r="C117" s="6"/>
+      <c r="D117" s="6"/>
+      <c r="E117" s="6"/>
+      <c r="F117" s="6"/>
+      <c r="G117" s="6"/>
+      <c r="H117" s="6"/>
     </row>
     <row r="118" spans="1:8">
       <c r="A118">
@@ -2529,6 +2601,784 @@
         <v>19</v>
       </c>
       <c r="H118" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="139" spans="2:2">
+      <c r="B139" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="140" spans="2:2">
+      <c r="B140" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="141" spans="2:2">
+      <c r="B141" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="142" spans="2:2">
+      <c r="B142" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="144" customFormat="1" spans="2:3">
+      <c r="B144" t="s">
+        <v>10</v>
+      </c>
+      <c r="C144" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="145" spans="3:8">
+      <c r="C145" t="s">
+        <v>12</v>
+      </c>
+      <c r="D145" t="s">
+        <v>13</v>
+      </c>
+      <c r="E145" t="s">
+        <v>14</v>
+      </c>
+      <c r="F145" t="s">
+        <v>15</v>
+      </c>
+      <c r="G145" t="s">
+        <v>16</v>
+      </c>
+      <c r="H145" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="146" customFormat="1"/>
+    <row r="147" spans="1:8">
+      <c r="A147">
+        <v>31</v>
+      </c>
+      <c r="B147" t="s">
+        <v>18</v>
+      </c>
+      <c r="C147" t="s">
+        <v>19</v>
+      </c>
+      <c r="D147" t="s">
+        <v>19</v>
+      </c>
+      <c r="E147" t="s">
+        <v>19</v>
+      </c>
+      <c r="F147" t="s">
+        <v>19</v>
+      </c>
+      <c r="G147" t="s">
+        <v>19</v>
+      </c>
+      <c r="H147" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="148" customFormat="1"/>
+    <row r="149" customFormat="1" spans="3:3">
+      <c r="C149" s="2"/>
+    </row>
+    <row r="150" spans="1:8">
+      <c r="A150">
+        <v>46</v>
+      </c>
+      <c r="B150" t="s">
+        <v>85</v>
+      </c>
+      <c r="C150" t="s">
+        <v>86</v>
+      </c>
+      <c r="D150" t="s">
+        <v>63</v>
+      </c>
+      <c r="E150" t="s">
+        <v>63</v>
+      </c>
+      <c r="F150" t="s">
+        <v>87</v>
+      </c>
+      <c r="G150" t="s">
+        <v>63</v>
+      </c>
+      <c r="H150" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="151" spans="3:8">
+      <c r="C151" s="3"/>
+      <c r="D151" s="3"/>
+      <c r="E151"/>
+      <c r="F151" s="3"/>
+      <c r="G151"/>
+      <c r="H151" s="3"/>
+    </row>
+    <row r="152" spans="1:8">
+      <c r="A152">
+        <v>47</v>
+      </c>
+      <c r="B152" t="s">
+        <v>88</v>
+      </c>
+      <c r="C152" t="s">
+        <v>89</v>
+      </c>
+      <c r="D152" t="s">
+        <v>61</v>
+      </c>
+      <c r="E152" t="s">
+        <v>63</v>
+      </c>
+      <c r="F152" t="s">
+        <v>90</v>
+      </c>
+      <c r="G152" t="s">
+        <v>63</v>
+      </c>
+      <c r="H152" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="153" spans="3:7">
+      <c r="C153" s="1"/>
+      <c r="D153"/>
+      <c r="E153" s="1"/>
+      <c r="F153"/>
+      <c r="G153" s="1"/>
+    </row>
+    <row r="154" spans="1:8">
+      <c r="A154">
+        <v>48</v>
+      </c>
+      <c r="B154" t="s">
+        <v>91</v>
+      </c>
+      <c r="C154" t="s">
+        <v>87</v>
+      </c>
+      <c r="D154" t="s">
+        <v>61</v>
+      </c>
+      <c r="E154" t="s">
+        <v>92</v>
+      </c>
+      <c r="F154" t="s">
+        <v>90</v>
+      </c>
+      <c r="G154" t="s">
+        <v>93</v>
+      </c>
+      <c r="H154" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="155" spans="4:8">
+      <c r="D155" s="3"/>
+      <c r="E155"/>
+      <c r="F155" s="3"/>
+      <c r="G155"/>
+      <c r="H155" s="3"/>
+    </row>
+    <row r="156" spans="1:8">
+      <c r="A156">
+        <v>49</v>
+      </c>
+      <c r="B156" t="s">
+        <v>94</v>
+      </c>
+      <c r="C156" t="s">
+        <v>87</v>
+      </c>
+      <c r="D156" t="s">
+        <v>63</v>
+      </c>
+      <c r="E156" t="s">
+        <v>92</v>
+      </c>
+      <c r="F156" t="s">
+        <v>87</v>
+      </c>
+      <c r="G156" t="s">
+        <v>93</v>
+      </c>
+      <c r="H156" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="157" spans="3:7">
+      <c r="C157" s="3"/>
+      <c r="D157"/>
+      <c r="E157" s="2"/>
+      <c r="F157"/>
+      <c r="G157" s="2"/>
+    </row>
+    <row r="158" spans="1:8">
+      <c r="A158">
+        <v>50</v>
+      </c>
+      <c r="B158" t="s">
+        <v>95</v>
+      </c>
+      <c r="C158" t="s">
+        <v>90</v>
+      </c>
+      <c r="D158" t="s">
+        <v>63</v>
+      </c>
+      <c r="E158" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F158" t="s">
+        <v>87</v>
+      </c>
+      <c r="G158" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H158" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="159" spans="4:8">
+      <c r="D159" s="1"/>
+      <c r="E159"/>
+      <c r="F159" s="1"/>
+      <c r="G159"/>
+      <c r="H159" s="1"/>
+    </row>
+    <row r="160" spans="1:8">
+      <c r="A160">
+        <v>51</v>
+      </c>
+      <c r="B160" t="s">
+        <v>96</v>
+      </c>
+      <c r="C160" t="s">
+        <v>90</v>
+      </c>
+      <c r="D160" t="s">
+        <v>92</v>
+      </c>
+      <c r="E160" t="s">
+        <v>61</v>
+      </c>
+      <c r="F160" t="s">
+        <v>89</v>
+      </c>
+      <c r="G160" t="s">
+        <v>61</v>
+      </c>
+      <c r="H160" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="161" spans="3:7">
+      <c r="C161" s="3"/>
+      <c r="D161"/>
+      <c r="E161" s="3"/>
+      <c r="F161"/>
+      <c r="G161" s="3"/>
+    </row>
+    <row r="162" spans="1:8">
+      <c r="A162">
+        <v>52</v>
+      </c>
+      <c r="B162" t="s">
+        <v>97</v>
+      </c>
+      <c r="C162" t="s">
+        <v>87</v>
+      </c>
+      <c r="D162" t="s">
+        <v>92</v>
+      </c>
+      <c r="E162" t="s">
+        <v>63</v>
+      </c>
+      <c r="F162" t="s">
+        <v>89</v>
+      </c>
+      <c r="G162" t="s">
+        <v>63</v>
+      </c>
+      <c r="H162" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="163" spans="4:8">
+      <c r="D163" s="2"/>
+      <c r="E163"/>
+      <c r="F163" s="2"/>
+      <c r="G163"/>
+      <c r="H163" s="2"/>
+    </row>
+    <row r="164" spans="1:8">
+      <c r="A164">
+        <v>53</v>
+      </c>
+      <c r="B164" t="s">
+        <v>98</v>
+      </c>
+      <c r="C164" t="s">
+        <v>87</v>
+      </c>
+      <c r="D164" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E164" t="s">
+        <v>63</v>
+      </c>
+      <c r="F164" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G164" t="s">
+        <v>63</v>
+      </c>
+      <c r="H164" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="165" spans="4:8">
+      <c r="D165" s="3"/>
+      <c r="E165"/>
+      <c r="F165" s="3"/>
+      <c r="G165"/>
+      <c r="H165" s="3"/>
+    </row>
+    <row r="167" spans="1:8">
+      <c r="A167">
+        <v>31</v>
+      </c>
+      <c r="B167" t="s">
+        <v>18</v>
+      </c>
+      <c r="C167" t="s">
+        <v>19</v>
+      </c>
+      <c r="D167" t="s">
+        <v>19</v>
+      </c>
+      <c r="E167" t="s">
+        <v>19</v>
+      </c>
+      <c r="F167" t="s">
+        <v>19</v>
+      </c>
+      <c r="G167" t="s">
+        <v>19</v>
+      </c>
+      <c r="H167" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="170" customFormat="1"/>
+    <row r="180" spans="2:2">
+      <c r="B180" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="181" customFormat="1" spans="2:2">
+      <c r="B181" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="182" customFormat="1" spans="2:2">
+      <c r="B182" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="183" customFormat="1" spans="2:2">
+      <c r="B183" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="184" customFormat="1" spans="2:2">
+      <c r="B184" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="185" customFormat="1" spans="2:2">
+      <c r="B185" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="186" customFormat="1" spans="2:3">
+      <c r="B186" t="s">
+        <v>10</v>
+      </c>
+      <c r="C186" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="187" spans="3:8">
+      <c r="C187" t="s">
+        <v>12</v>
+      </c>
+      <c r="D187" t="s">
+        <v>13</v>
+      </c>
+      <c r="E187" t="s">
+        <v>14</v>
+      </c>
+      <c r="F187" t="s">
+        <v>15</v>
+      </c>
+      <c r="G187" t="s">
+        <v>16</v>
+      </c>
+      <c r="H187" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="188" customFormat="1"/>
+    <row r="189" spans="1:8">
+      <c r="A189">
+        <v>31</v>
+      </c>
+      <c r="B189" t="s">
+        <v>18</v>
+      </c>
+      <c r="C189" t="s">
+        <v>19</v>
+      </c>
+      <c r="D189" t="s">
+        <v>19</v>
+      </c>
+      <c r="E189" t="s">
+        <v>19</v>
+      </c>
+      <c r="F189" t="s">
+        <v>19</v>
+      </c>
+      <c r="G189" t="s">
+        <v>19</v>
+      </c>
+      <c r="H189" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="190" customFormat="1"/>
+    <row r="192" customFormat="1" spans="1:8">
+      <c r="A192">
+        <v>53</v>
+      </c>
+      <c r="B192" t="s">
+        <v>104</v>
+      </c>
+      <c r="C192" t="s">
+        <v>61</v>
+      </c>
+      <c r="D192" t="s">
+        <v>87</v>
+      </c>
+      <c r="E192" t="s">
+        <v>61</v>
+      </c>
+      <c r="F192" t="s">
+        <v>63</v>
+      </c>
+      <c r="G192" t="s">
+        <v>90</v>
+      </c>
+      <c r="H192" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="193" spans="3:8">
+      <c r="C193" s="2"/>
+      <c r="D193" s="1"/>
+      <c r="E193" s="2"/>
+      <c r="F193" s="1"/>
+      <c r="G193" s="2"/>
+      <c r="H193" s="1"/>
+    </row>
+    <row r="194" spans="1:8">
+      <c r="A194">
+        <v>46</v>
+      </c>
+      <c r="B194" t="s">
+        <v>105</v>
+      </c>
+      <c r="C194" t="s">
+        <v>106</v>
+      </c>
+      <c r="D194" t="s">
+        <v>107</v>
+      </c>
+      <c r="E194" t="s">
+        <v>108</v>
+      </c>
+      <c r="F194" t="s">
+        <v>109</v>
+      </c>
+      <c r="G194" t="s">
+        <v>86</v>
+      </c>
+      <c r="H194" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="195" spans="3:7">
+      <c r="C195" s="3"/>
+      <c r="D195"/>
+      <c r="E195" s="3"/>
+      <c r="G195" s="3"/>
+    </row>
+    <row r="196" spans="1:8">
+      <c r="A196">
+        <v>47</v>
+      </c>
+      <c r="B196" t="s">
+        <v>111</v>
+      </c>
+      <c r="C196" t="s">
+        <v>109</v>
+      </c>
+      <c r="D196" t="s">
+        <v>107</v>
+      </c>
+      <c r="E196" t="s">
+        <v>110</v>
+      </c>
+      <c r="F196" t="s">
+        <v>109</v>
+      </c>
+      <c r="G196" t="s">
+        <v>89</v>
+      </c>
+      <c r="H196" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="197" customFormat="1" spans="4:8">
+      <c r="D197" s="3"/>
+      <c r="E197"/>
+      <c r="F197" s="3"/>
+      <c r="G197"/>
+      <c r="H197" s="3"/>
+    </row>
+    <row r="198" spans="1:8">
+      <c r="A198">
+        <v>48</v>
+      </c>
+      <c r="B198" t="s">
+        <v>112</v>
+      </c>
+      <c r="C198" t="s">
+        <v>109</v>
+      </c>
+      <c r="D198" t="s">
+        <v>113</v>
+      </c>
+      <c r="E198" t="s">
+        <v>110</v>
+      </c>
+      <c r="F198" t="s">
+        <v>106</v>
+      </c>
+      <c r="G198" t="s">
+        <v>89</v>
+      </c>
+      <c r="H198" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="199" spans="3:8">
+      <c r="C199" s="1"/>
+      <c r="D199" s="2"/>
+      <c r="E199" s="1"/>
+      <c r="F199" s="2"/>
+      <c r="G199" s="1"/>
+      <c r="H199" s="2"/>
+    </row>
+    <row r="200" spans="1:8">
+      <c r="A200">
+        <v>49</v>
+      </c>
+      <c r="B200" t="s">
+        <v>114</v>
+      </c>
+      <c r="C200" t="s">
+        <v>63</v>
+      </c>
+      <c r="D200" t="s">
+        <v>90</v>
+      </c>
+      <c r="E200" t="s">
+        <v>63</v>
+      </c>
+      <c r="F200" t="s">
+        <v>61</v>
+      </c>
+      <c r="G200" t="s">
+        <v>87</v>
+      </c>
+      <c r="H200" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="201" customFormat="1" spans="3:8">
+      <c r="C201" s="1"/>
+      <c r="D201" s="2"/>
+      <c r="E201" s="1"/>
+      <c r="F201" s="2"/>
+      <c r="G201" s="1"/>
+      <c r="H201" s="2"/>
+    </row>
+    <row r="202" spans="1:8">
+      <c r="A202">
+        <v>50</v>
+      </c>
+      <c r="B202" t="s">
+        <v>115</v>
+      </c>
+      <c r="C202" t="s">
+        <v>116</v>
+      </c>
+      <c r="D202" t="s">
+        <v>86</v>
+      </c>
+      <c r="E202" t="s">
+        <v>117</v>
+      </c>
+      <c r="F202" t="s">
+        <v>118</v>
+      </c>
+      <c r="G202" t="s">
+        <v>107</v>
+      </c>
+      <c r="H202" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="203" spans="4:8">
+      <c r="D203" s="3"/>
+      <c r="E203"/>
+      <c r="F203" s="3"/>
+      <c r="G203"/>
+      <c r="H203" s="3"/>
+    </row>
+    <row r="204" spans="1:8">
+      <c r="A204">
+        <v>51</v>
+      </c>
+      <c r="B204" t="s">
+        <v>120</v>
+      </c>
+      <c r="C204" t="s">
+        <v>116</v>
+      </c>
+      <c r="D204" t="s">
+        <v>121</v>
+      </c>
+      <c r="E204" t="s">
+        <v>117</v>
+      </c>
+      <c r="F204" t="s">
+        <v>116</v>
+      </c>
+      <c r="G204" t="s">
+        <v>107</v>
+      </c>
+      <c r="H204" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="205" customFormat="1" spans="3:7">
+      <c r="C205" s="3"/>
+      <c r="D205"/>
+      <c r="E205" s="3"/>
+      <c r="F205"/>
+      <c r="G205" s="3"/>
+    </row>
+    <row r="206" spans="1:8">
+      <c r="A206">
+        <v>52</v>
+      </c>
+      <c r="B206" t="s">
+        <v>122</v>
+      </c>
+      <c r="C206" t="s">
+        <v>118</v>
+      </c>
+      <c r="D206" t="s">
+        <v>121</v>
+      </c>
+      <c r="E206" t="s">
+        <v>119</v>
+      </c>
+      <c r="F206" t="s">
+        <v>116</v>
+      </c>
+      <c r="G206" t="s">
+        <v>113</v>
+      </c>
+      <c r="H206" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="207" customFormat="1" spans="3:8">
+      <c r="C207" s="2"/>
+      <c r="D207" s="1"/>
+      <c r="E207" s="2"/>
+      <c r="F207" s="1"/>
+      <c r="G207" s="2"/>
+      <c r="H207" s="1"/>
+    </row>
+    <row r="208" spans="1:8">
+      <c r="A208">
+        <v>53</v>
+      </c>
+      <c r="B208" t="s">
+        <v>104</v>
+      </c>
+      <c r="C208" t="s">
+        <v>61</v>
+      </c>
+      <c r="D208" t="s">
+        <v>87</v>
+      </c>
+      <c r="E208" t="s">
+        <v>61</v>
+      </c>
+      <c r="F208" t="s">
+        <v>63</v>
+      </c>
+      <c r="G208" t="s">
+        <v>90</v>
+      </c>
+      <c r="H208" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="209" customFormat="1"/>
+    <row r="210" customFormat="1"/>
+    <row r="211" spans="1:8">
+      <c r="A211">
+        <v>31</v>
+      </c>
+      <c r="B211" t="s">
+        <v>18</v>
+      </c>
+      <c r="C211" t="s">
+        <v>19</v>
+      </c>
+      <c r="D211" t="s">
+        <v>19</v>
+      </c>
+      <c r="E211" t="s">
+        <v>19</v>
+      </c>
+      <c r="F211" t="s">
+        <v>19</v>
+      </c>
+      <c r="G211" t="s">
+        <v>19</v>
+      </c>
+      <c r="H211" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>